<commit_message>
Added Suit and listener
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/OrangeHRM.xlsx
+++ b/src/test/resources/ExcelData/OrangeHRM.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14340" windowHeight="6435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>Email</t>
   </si>
@@ -24,34 +25,23 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Nagesh</t>
+    <t>Admin</t>
   </si>
   <si>
-    <t>abc@123</t>
+    <t>admin123</t>
   </si>
   <si>
-    <t>MohiniVaswade</t>
-  </si>
-  <si>
-    <t>"  "</t>
+    <t>""</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -74,16 +64,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -383,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,22 +390,35 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>